<commit_message>
Gold API Login and workspace method
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API/GoldApiTestData.xlsx
+++ b/src/test/resources/TestData/API/GoldApiTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BE49F8-9604-49EB-ADE5-0B2D93E2DFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B56FA6-4256-4C51-9007-C5EF58D1B276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="229">
   <si>
     <t>UserName</t>
   </si>
@@ -728,6 +728,12 @@
   </si>
   <si>
     <t>00622</t>
+  </si>
+  <si>
+    <t>Post_Account</t>
+  </si>
+  <si>
+    <t>magentoapi123</t>
   </si>
 </sst>
 </file>
@@ -1159,19 +1165,19 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1244,7 +1250,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1254,63 +1260,63 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" s="6"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="7"/>
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
@@ -1332,13 +1338,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -1420,13 +1426,13 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1439,7 +1445,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1467,23 +1473,23 @@
       <selection activeCell="I2" sqref="I2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1638,7 +1644,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="9"/>
     </row>
   </sheetData>
@@ -1712,21 +1718,21 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="44.7109375" customWidth="1"/>
+    <col min="14" max="14" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.6640625" customWidth="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1800,7 +1806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1894,33 +1900,33 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="11" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.42578125" customWidth="1"/>
-    <col min="43" max="43" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.44140625" customWidth="1"/>
+    <col min="43" max="43" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2148,7 +2154,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2170,7 +2176,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2198,7 +2204,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2212,7 +2218,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2283,7 +2289,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -2313,7 +2319,7 @@
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -2344,7 +2350,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -2376,7 +2382,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -2435,7 +2441,7 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="5"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -2492,7 +2498,7 @@
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2568,7 +2574,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -2582,7 +2588,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -2634,15 +2640,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C559D8FD-F843-407C-919F-478081CBDB61}">
-  <dimension ref="A1:AJ40"/>
+  <dimension ref="A1:AJ41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2808,113 +2814,117 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
-      <c r="R3" t="s">
-        <v>185</v>
-      </c>
-      <c r="S3" t="s">
-        <v>186</v>
-      </c>
-      <c r="T3" t="s">
-        <v>187</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
-      <c r="X4" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z4" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>185</v>
+      </c>
+      <c r="S4" t="s">
+        <v>186</v>
+      </c>
+      <c r="T4" t="s">
+        <v>187</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>179</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="X5" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="Y5" t="s">
-        <v>192</v>
+        <v>137</v>
       </c>
       <c r="Z5" s="7" t="s">
         <v>189</v>
       </c>
+      <c r="AA5" t="s">
+        <v>46</v>
+      </c>
       <c r="AB5" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="X6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Y6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Z6" s="7" t="s">
         <v>189</v>
@@ -2923,135 +2933,138 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>196</v>
-      </c>
-      <c r="C7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D7" t="s">
-        <v>196</v>
-      </c>
-      <c r="L7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" t="s">
-        <v>43</v>
+        <v>193</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
-      <c r="R7" t="s">
-        <v>180</v>
-      </c>
-      <c r="S7" t="s">
-        <v>181</v>
-      </c>
-      <c r="T7" t="s">
-        <v>182</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC7" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="X7" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="2"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AC8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>180</v>
+      </c>
+      <c r="S8" t="s">
+        <v>181</v>
+      </c>
+      <c r="T8" t="s">
+        <v>182</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>48</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-      <c r="AD9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF9">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R9" s="2"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AC9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="AD10" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AE10" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AF10">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="AD11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE11" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AF11">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="AD12" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AE12" s="5" t="s">
         <v>50</v>
@@ -3060,47 +3073,46 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AD13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="M14" t="s">
         <v>32</v>
@@ -3109,129 +3121,117 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="2"/>
-      <c r="S14" t="s">
-        <v>181</v>
-      </c>
-      <c r="T14" t="s">
-        <v>182</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="L15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15" t="s">
+        <v>32</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
-      <c r="AD15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R15" s="2"/>
+      <c r="S15" t="s">
+        <v>181</v>
+      </c>
+      <c r="T15" t="s">
+        <v>182</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="W15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="2"/>
+        <v>59</v>
+      </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="2"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AC16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AD16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>168</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>178</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="M17" s="8"/>
+      <c r="E17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="2"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
-      <c r="R17" s="8"/>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R17" s="2"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AC17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>80</v>
-      </c>
-      <c r="L18" t="s">
-        <v>32</v>
-      </c>
-      <c r="M18" t="s">
-        <v>43</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="M18" s="8"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
-      <c r="R18" t="s">
-        <v>201</v>
-      </c>
-      <c r="S18" t="s">
-        <v>202</v>
-      </c>
-      <c r="T18" t="s">
-        <v>203</v>
-      </c>
-      <c r="U18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="W18" s="3"/>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R18" s="8"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>80</v>
       </c>
       <c r="L19" t="s">
         <v>32</v>
@@ -3244,44 +3244,26 @@
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="S19" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="T19" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="V19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
+        <v>204</v>
+      </c>
       <c r="L20" t="s">
         <v>32</v>
       </c>
@@ -3293,37 +3275,34 @@
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="S20" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="T20" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="W20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="5"/>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="7" t="s">
@@ -3345,259 +3324,286 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="T21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="V21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="Z21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="5"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>87</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" t="s">
+        <v>43</v>
       </c>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
-      <c r="X22" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z22" s="3"/>
-      <c r="AB22" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>89</v>
+      </c>
+      <c r="S22" t="s">
+        <v>90</v>
+      </c>
+      <c r="T22" t="s">
+        <v>91</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
-      <c r="AC23" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="X23" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z23" s="3"/>
+      <c r="AB23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="J24" t="s">
-        <v>209</v>
-      </c>
-      <c r="L24" t="s">
-        <v>32</v>
-      </c>
-      <c r="M24" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
-      <c r="AG24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AC24" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>99</v>
+      </c>
+      <c r="J25" t="s">
+        <v>209</v>
+      </c>
+      <c r="L25" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" t="s">
+        <v>43</v>
       </c>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
-      <c r="AB25" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AG25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="J26" s="3"/>
-      <c r="K26" t="s">
-        <v>210</v>
+        <v>42</v>
       </c>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AB26" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="J27" t="s">
-        <v>211</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" t="s">
+        <v>210</v>
+      </c>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>124</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="I28" t="s">
+        <v>179</v>
+      </c>
+      <c r="J28" t="s">
+        <v>211</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
-      <c r="AH28" t="s">
-        <v>212</v>
-      </c>
-      <c r="AI28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
-      <c r="X29" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>140</v>
+      <c r="AH29" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>138</v>
       </c>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="X30" s="16" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I31" t="s">
-        <v>179</v>
-      </c>
-      <c r="L31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M31" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
-      <c r="R31" t="s">
-        <v>180</v>
-      </c>
-      <c r="S31" t="s">
-        <v>181</v>
-      </c>
-      <c r="T31" t="s">
-        <v>182</v>
-      </c>
-      <c r="U31" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="V31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="W31" s="3">
-        <v>888888</v>
-      </c>
-      <c r="Y31" s="17">
-        <v>32725</v>
-      </c>
-      <c r="AD31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF31">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="X31" s="16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>62</v>
+        <v>141</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" t="s">
+        <v>179</v>
+      </c>
+      <c r="L32" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" t="s">
+        <v>31</v>
       </c>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="R32" t="s">
+        <v>180</v>
+      </c>
+      <c r="S32" t="s">
+        <v>181</v>
+      </c>
+      <c r="T32" t="s">
+        <v>182</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W32" s="3">
+        <v>888888</v>
+      </c>
+      <c r="Y32" s="17">
+        <v>32725</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF32">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="18"/>
+        <v>143</v>
+      </c>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>160</v>
@@ -3611,104 +3617,129 @@
       <c r="E35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="L35" t="s">
-        <v>94</v>
-      </c>
-      <c r="M35" t="s">
-        <v>39</v>
-      </c>
-      <c r="N35" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="O35" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="P35" s="19">
-        <v>4</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F35" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="18"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>216</v>
+        <v>152</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="L36" t="s">
+        <v>94</v>
+      </c>
+      <c r="M36" t="s">
+        <v>39</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="P36" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="F37" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="AC37" s="3" t="s">
+      <c r="AC38" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="AC38" s="3" t="s">
+      <c r="AC39" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="AC39" s="3" t="s">
+      <c r="AC40" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L41" t="s">
         <v>32</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M41" t="s">
         <v>31</v>
       </c>
-      <c r="R40" t="s">
+      <c r="R41" t="s">
         <v>223</v>
       </c>
-      <c r="S40" t="s">
+      <c r="S41" t="s">
         <v>224</v>
       </c>
-      <c r="T40" t="s">
+      <c r="T41" t="s">
         <v>225</v>
       </c>
-      <c r="U40" s="3" t="s">
+      <c r="U41" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="V40" s="3" t="s">
+      <c r="V41" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3718,38 +3749,39 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{16136D4B-E0DF-4DB2-B4D1-ABF0F2B7CA08}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{8FE9EB04-F6C1-4AA9-8202-6D18E322DE03}"/>
     <hyperlink ref="C2" r:id="rId4" display="testersemail.278@gmail.com" xr:uid="{C7FCAAA6-C5F4-4E23-BEE6-5E2DBC6AF4FF}"/>
-    <hyperlink ref="E13" r:id="rId5" xr:uid="{ACCA61CA-C66C-4251-858A-0373AF6D3512}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{74356F15-E3CE-4806-840C-A65CA38C5CEC}"/>
-    <hyperlink ref="C16" r:id="rId7" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
-    <hyperlink ref="C17" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
-    <hyperlink ref="F17" r:id="rId9" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
-    <hyperlink ref="B20" r:id="rId11" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
-    <hyperlink ref="C20" r:id="rId12" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
-    <hyperlink ref="B13" r:id="rId13" display="mailto:hmaram@helenoftroy.com" xr:uid="{2B07C3A2-6123-45F7-BC86-05D1271EEC94}"/>
+    <hyperlink ref="E14" r:id="rId5" xr:uid="{ACCA61CA-C66C-4251-858A-0373AF6D3512}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{74356F15-E3CE-4806-840C-A65CA38C5CEC}"/>
+    <hyperlink ref="C17" r:id="rId7" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
+    <hyperlink ref="C18" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
+    <hyperlink ref="E22" r:id="rId10" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
+    <hyperlink ref="B21" r:id="rId11" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
+    <hyperlink ref="C21" r:id="rId12" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
+    <hyperlink ref="B14" r:id="rId13" display="mailto:hmaram@helenoftroy.com" xr:uid="{2B07C3A2-6123-45F7-BC86-05D1271EEC94}"/>
     <hyperlink ref="D2" r:id="rId14" display="testersemail.278@gmail.com" xr:uid="{353015EC-BFE3-4FB0-A1D6-8368DFF2AD28}"/>
-    <hyperlink ref="B34" r:id="rId15" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
-    <hyperlink ref="C34" r:id="rId16" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
-    <hyperlink ref="D34" r:id="rId17" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
-    <hyperlink ref="E34" r:id="rId18" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
-    <hyperlink ref="B35" r:id="rId19" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
-    <hyperlink ref="C35" r:id="rId20" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
-    <hyperlink ref="D35" r:id="rId21" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
-    <hyperlink ref="E35" r:id="rId22" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
-    <hyperlink ref="C31" r:id="rId23" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
-    <hyperlink ref="B36" r:id="rId24" xr:uid="{3269489F-E375-4158-9D38-F364B85C1533}"/>
-    <hyperlink ref="C36" r:id="rId25" xr:uid="{2554AE08-E4AE-498E-A4A1-E24F8975ECB8}"/>
-    <hyperlink ref="D36" r:id="rId26" xr:uid="{93AB37E3-19EA-44E4-B2EC-0BD928ADFE48}"/>
-    <hyperlink ref="E36" r:id="rId27" xr:uid="{D81BF4A4-1FDA-4D9E-A6CD-BCCC895D2A97}"/>
-    <hyperlink ref="F36" r:id="rId28" xr:uid="{07D244B4-46C0-4B73-998C-F9B2F7C6345C}"/>
-    <hyperlink ref="B40" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{1573A67E-2555-410F-9BD0-669B1EB48FA8}"/>
-    <hyperlink ref="C40" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{BE3AE9D2-A787-4116-82BC-B575A94256FD}"/>
-    <hyperlink ref="D40" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{1252E651-EBF0-4B6A-8D9E-948ACC0F9294}"/>
-    <hyperlink ref="B17" r:id="rId32" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
-    <hyperlink ref="C8" r:id="rId33" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
-    <hyperlink ref="B3" r:id="rId34" xr:uid="{77E09AB9-2BDE-4CFC-B912-232E3CA6F93A}"/>
-    <hyperlink ref="C3" r:id="rId35" xr:uid="{7526D2B7-3779-4673-A300-D16AD3913B73}"/>
-    <hyperlink ref="D3" r:id="rId36" xr:uid="{D01B3849-C5F1-4873-9AE5-D6B5A87C0C9A}"/>
+    <hyperlink ref="B35" r:id="rId15" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
+    <hyperlink ref="C35" r:id="rId16" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
+    <hyperlink ref="D35" r:id="rId17" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
+    <hyperlink ref="E35" r:id="rId18" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
+    <hyperlink ref="B36" r:id="rId19" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
+    <hyperlink ref="C36" r:id="rId20" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
+    <hyperlink ref="D36" r:id="rId21" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
+    <hyperlink ref="E36" r:id="rId22" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
+    <hyperlink ref="C32" r:id="rId23" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
+    <hyperlink ref="B37" r:id="rId24" xr:uid="{3269489F-E375-4158-9D38-F364B85C1533}"/>
+    <hyperlink ref="C37" r:id="rId25" xr:uid="{2554AE08-E4AE-498E-A4A1-E24F8975ECB8}"/>
+    <hyperlink ref="D37" r:id="rId26" xr:uid="{93AB37E3-19EA-44E4-B2EC-0BD928ADFE48}"/>
+    <hyperlink ref="E37" r:id="rId27" xr:uid="{D81BF4A4-1FDA-4D9E-A6CD-BCCC895D2A97}"/>
+    <hyperlink ref="F37" r:id="rId28" xr:uid="{07D244B4-46C0-4B73-998C-F9B2F7C6345C}"/>
+    <hyperlink ref="B41" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{1573A67E-2555-410F-9BD0-669B1EB48FA8}"/>
+    <hyperlink ref="C41" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{BE3AE9D2-A787-4116-82BC-B575A94256FD}"/>
+    <hyperlink ref="D41" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{1252E651-EBF0-4B6A-8D9E-948ACC0F9294}"/>
+    <hyperlink ref="B18" r:id="rId32" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
+    <hyperlink ref="C9" r:id="rId33" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
+    <hyperlink ref="B4" r:id="rId34" xr:uid="{77E09AB9-2BDE-4CFC-B912-232E3CA6F93A}"/>
+    <hyperlink ref="C4" r:id="rId35" xr:uid="{7526D2B7-3779-4673-A300-D16AD3913B73}"/>
+    <hyperlink ref="D4" r:id="rId36" xr:uid="{D01B3849-C5F1-4873-9AE5-D6B5A87C0C9A}"/>
+    <hyperlink ref="B3" r:id="rId37" xr:uid="{D8EBB8AF-0E4E-43B7-9BD6-9022D3DBD128}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Api Token changes for osprey us
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API/GoldApiTestData.xlsx
+++ b/src/test/resources/TestData/API/GoldApiTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F96B9D-421E-4E0F-A44D-32EEFC98344A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7627A8-4A4A-4A58-BA1B-1783C7ABA6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -724,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -740,6 +740,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1943,7 +1944,7 @@
   <dimension ref="A1:AO33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,7 +2219,7 @@
       <c r="H5" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="15" t="s">
         <v>189</v>
       </c>
       <c r="J5" s="2" t="s">

</xml_diff>

<commit_message>
Api code changes for authorization token
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API/GoldApiTestData.xlsx
+++ b/src/test/resources/TestData/API/GoldApiTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7627A8-4A4A-4A58-BA1B-1783C7ABA6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C16701-11FE-484D-BA89-4E49819F9D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2496" yWindow="2496" windowWidth="17280" windowHeight="9108" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="205">
   <si>
     <t>UserName</t>
   </si>
@@ -591,9 +591,6 @@
     <t>Token</t>
   </si>
   <si>
-    <t>https://na-preprod.hele.digital/rest/V1/integration/admin/token</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
@@ -619,6 +616,27 @@
   </si>
   <si>
     <t>https://na-preprod.hele.digital/heledigitaladmin/sales/order/view/order_id/</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Get Order</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>https://na-preprod.hele.digital/rest/ospreyusen/V1/orders/</t>
+  </si>
+  <si>
+    <t>hhttps://na-preprod.hele.digital/rest/V1/integration/admin/token</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>"</t>
   </si>
 </sst>
 </file>
@@ -724,7 +742,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -741,6 +759,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1028,19 +1047,19 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1103,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1098,7 +1117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1113,7 +1132,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1123,63 +1142,63 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" s="6"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="7"/>
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
@@ -1201,33 +1220,33 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="11" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.42578125" customWidth="1"/>
-    <col min="43" max="43" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.44140625" customWidth="1"/>
+    <col min="43" max="43" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1361,7 +1380,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1424,7 +1443,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1447,7 +1466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1455,7 +1474,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -1463,7 +1482,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1477,7 +1496,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1491,7 +1510,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1505,7 +1524,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1519,7 +1538,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1552,7 +1571,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1590,7 +1609,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1604,7 +1623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1620,7 +1639,7 @@
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1651,7 +1670,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1683,7 +1702,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1742,7 +1761,7 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="5"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1799,7 +1818,7 @@
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1811,7 +1830,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1819,7 +1838,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -1836,7 +1855,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1844,7 +1863,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1858,7 +1877,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1875,7 +1894,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1889,7 +1908,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1906,7 +1925,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -1941,28 +1960,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C559D8FD-F843-407C-919F-478081CBDB61}">
-  <dimension ref="A1:AO33"/>
+  <dimension ref="A1:AQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="60.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="60.88671875" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1982,112 +2001,118 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2113,42 +2138,44 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" t="s">
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" t="s">
         <v>155</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" t="s">
         <v>32</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
-      <c r="W2" t="s">
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" t="s">
         <v>156</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>158</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB2" s="3"/>
-      <c r="AO2" t="s">
+      <c r="AD2" s="3"/>
+      <c r="AQ2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>180</v>
       </c>
@@ -2168,17 +2195,19 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
       <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -2191,22 +2220,24 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
       <c r="U4" s="9"/>
       <c r="V4" s="9"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
       <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -2216,409 +2247,394 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="J5" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
       <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>141</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
       <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>191</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I7" s="7"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="7"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
       <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" t="s">
-        <v>155</v>
-      </c>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+        <v>196</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
-      <c r="AC8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE8" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG8" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R9" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="P9" t="s">
+        <v>155</v>
+      </c>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
-      <c r="W9" t="s">
-        <v>156</v>
-      </c>
-      <c r="X9" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH9" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="AE9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG9" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI9" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="S10" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" t="s">
+        <v>43</v>
+      </c>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
-      <c r="W10" s="2"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AH10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ10" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
+        <v>163</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T11" s="2"/>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
-      <c r="AI11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK11">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="2"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AJ11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
+        <v>48</v>
+      </c>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
-      <c r="AI12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ12" s="5" t="s">
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="AK12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AK12">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AM12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>53</v>
-      </c>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
+        <v>51</v>
+      </c>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
-      <c r="AI13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ13" s="5" t="s">
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="AK13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AK13">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AM13">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
+        <v>53</v>
+      </c>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
-      <c r="AI14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ14" s="5" t="s">
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="AK14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AK14">
+      <c r="AM14">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
+        <v>55</v>
+      </c>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
-      <c r="W15" s="2"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AH15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="AK15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
+      <c r="E16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T16" s="2"/>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="8"/>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="2"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AJ16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>32</v>
-      </c>
-      <c r="R17" t="s">
-        <v>43</v>
-      </c>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="T17" s="8"/>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
-      <c r="W17" t="s">
-        <v>166</v>
-      </c>
-      <c r="X17" t="s">
-        <v>167</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB17" s="3"/>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="8"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" t="s">
+        <v>74</v>
+      </c>
+      <c r="S18" t="s">
         <v>32</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>43</v>
       </c>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
-      <c r="W18" t="s">
-        <v>76</v>
-      </c>
-      <c r="X18" t="s">
-        <v>77</v>
-      </c>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
       <c r="Y18" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA18" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="5"/>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AD18" s="3"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -2634,275 +2650,306 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
-      <c r="Q19" t="s">
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" t="s">
         <v>32</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>43</v>
       </c>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
       <c r="U19" s="9"/>
       <c r="V19" s="9"/>
-      <c r="W19" t="s">
-        <v>82</v>
-      </c>
-      <c r="X19" t="s">
-        <v>83</v>
-      </c>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
       <c r="Y19" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AD19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="5"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" t="s">
+        <v>32</v>
+      </c>
+      <c r="T20" t="s">
+        <v>43</v>
+      </c>
       <c r="U20" s="9"/>
       <c r="V20" s="9"/>
-      <c r="AC20" t="s">
-        <v>171</v>
-      </c>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
-      <c r="AG20" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+        <v>86</v>
+      </c>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
-      <c r="AH21" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="AE21" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG21" s="3"/>
+      <c r="AI21" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>92</v>
-      </c>
-      <c r="O22" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>32</v>
-      </c>
-      <c r="R22" t="s">
-        <v>43</v>
-      </c>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+        <v>91</v>
+      </c>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
-      <c r="AL22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="AJ22" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
+        <v>92</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>173</v>
+      </c>
+      <c r="S23" t="s">
+        <v>32</v>
+      </c>
+      <c r="T23" t="s">
+        <v>43</v>
+      </c>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
-      <c r="AG23" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="AN23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="L24" t="s">
-        <v>97</v>
-      </c>
-      <c r="M24" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="O24" s="3"/>
-      <c r="P24" t="s">
-        <v>174</v>
-      </c>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
+        <v>42</v>
+      </c>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="AI24" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" t="s">
+        <v>29</v>
+      </c>
+      <c r="P25" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="O25" t="s">
-        <v>175</v>
-      </c>
-      <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
+      <c r="R25" t="s">
+        <v>174</v>
+      </c>
       <c r="U25" s="9"/>
       <c r="V25" s="9"/>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>108</v>
-      </c>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
+        <v>98</v>
+      </c>
+      <c r="P26" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>175</v>
+      </c>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
-      <c r="AM26" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+        <v>108</v>
+      </c>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
-      <c r="AC27" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="AO27" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
-      <c r="AC28" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="AE28" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N29" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>32</v>
-      </c>
-      <c r="R29" t="s">
-        <v>31</v>
-      </c>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+        <v>123</v>
+      </c>
       <c r="U29" s="9"/>
       <c r="V29" s="9"/>
-      <c r="W29" t="s">
-        <v>156</v>
-      </c>
-      <c r="X29" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z29" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AA29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB29" s="3">
-        <v>888888</v>
-      </c>
-      <c r="AD29" s="12">
-        <v>32725</v>
-      </c>
-      <c r="AI29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK29">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="AE29" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
+        <v>124</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P30" t="s">
+        <v>155</v>
+      </c>
+      <c r="S30" t="s">
+        <v>32</v>
+      </c>
+      <c r="T30" t="s">
+        <v>31</v>
+      </c>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB30" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>888888</v>
+      </c>
+      <c r="AF30" s="12">
+        <v>32725</v>
+      </c>
+      <c r="AK30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM30">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
+        <v>62</v>
+      </c>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
+        <v>126</v>
+      </c>
       <c r="U32" s="9"/>
       <c r="V32" s="9"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>143</v>
@@ -2916,61 +2963,96 @@
       <c r="E33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="Q33" t="s">
+      <c r="F33" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="S34" t="s">
         <v>87</v>
       </c>
-      <c r="R33" t="s">
+      <c r="T34" t="s">
         <v>39</v>
       </c>
-      <c r="S33" s="9" t="s">
+      <c r="U34" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="T33" s="9" t="s">
+      <c r="V34" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="U33" s="14">
+      <c r="W34" s="14">
         <v>4</v>
       </c>
-      <c r="V33" t="s">
+      <c r="X34" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D8EBB8AF-0E4E-43B7-9BD6-9022D3DBD128}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
-    <hyperlink ref="B16" r:id="rId3" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
-    <hyperlink ref="C29" r:id="rId4" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
-    <hyperlink ref="E33" r:id="rId5" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
-    <hyperlink ref="D33" r:id="rId6" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
-    <hyperlink ref="C33" r:id="rId7" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
-    <hyperlink ref="B33" r:id="rId8" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
-    <hyperlink ref="E32" r:id="rId9" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
-    <hyperlink ref="D32" r:id="rId10" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
-    <hyperlink ref="C32" r:id="rId11" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
-    <hyperlink ref="B32" r:id="rId12" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
+    <hyperlink ref="B17" r:id="rId3" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
+    <hyperlink ref="C30" r:id="rId4" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
+    <hyperlink ref="E34" r:id="rId5" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
+    <hyperlink ref="D34" r:id="rId6" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
+    <hyperlink ref="C34" r:id="rId7" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
+    <hyperlink ref="B34" r:id="rId8" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
+    <hyperlink ref="E33" r:id="rId9" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
+    <hyperlink ref="D33" r:id="rId10" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
+    <hyperlink ref="C33" r:id="rId11" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
+    <hyperlink ref="B33" r:id="rId12" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
     <hyperlink ref="D2" r:id="rId13" display="testersemail.278@gmail.com" xr:uid="{353015EC-BFE3-4FB0-A1D6-8368DFF2AD28}"/>
-    <hyperlink ref="C18" r:id="rId14" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
-    <hyperlink ref="B18" r:id="rId15" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
-    <hyperlink ref="F16" r:id="rId17" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
-    <hyperlink ref="C16" r:id="rId18" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
-    <hyperlink ref="C15" r:id="rId19" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
+    <hyperlink ref="C19" r:id="rId14" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
+    <hyperlink ref="B19" r:id="rId15" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
+    <hyperlink ref="E20" r:id="rId16" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
+    <hyperlink ref="F17" r:id="rId17" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
+    <hyperlink ref="C17" r:id="rId18" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
+    <hyperlink ref="C16" r:id="rId19" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
     <hyperlink ref="C2" r:id="rId20" display="testersemail.278@gmail.com" xr:uid="{C7FCAAA6-C5F4-4E23-BEE6-5E2DBC6AF4FF}"/>
     <hyperlink ref="F2" r:id="rId21" xr:uid="{8FE9EB04-F6C1-4AA9-8202-6D18E322DE03}"/>
     <hyperlink ref="E2" r:id="rId22" xr:uid="{16136D4B-E0DF-4DB2-B4D1-ABF0F2B7CA08}"/>
     <hyperlink ref="B2" r:id="rId23" xr:uid="{16F2B5CD-2E1E-47F3-B21F-B0588CAC3B53}"/>
-    <hyperlink ref="I5" r:id="rId24" xr:uid="{B8077304-30B9-4A5C-85B3-A0C1F75FD2D9}"/>
-    <hyperlink ref="B6" r:id="rId25" xr:uid="{3B86B051-3E41-4698-9B88-E4A853158AAD}"/>
-    <hyperlink ref="G6" r:id="rId26" xr:uid="{3EC40F05-66F6-4B2B-8CD2-3C51732A9D4D}"/>
-    <hyperlink ref="G7" r:id="rId27" xr:uid="{C892FDEA-8590-4AC0-9C8F-5B938B91B017}"/>
+    <hyperlink ref="J5" r:id="rId24" display="https://na-preprod.hele.digital/rest/V1/integration/admin/token" xr:uid="{B8077304-30B9-4A5C-85B3-A0C1F75FD2D9}"/>
+    <hyperlink ref="B7" r:id="rId25" xr:uid="{3B86B051-3E41-4698-9B88-E4A853158AAD}"/>
+    <hyperlink ref="H7" r:id="rId26" xr:uid="{3EC40F05-66F6-4B2B-8CD2-3C51732A9D4D}"/>
+    <hyperlink ref="H8" r:id="rId27" xr:uid="{C892FDEA-8590-4AC0-9C8F-5B938B91B017}"/>
+    <hyperlink ref="H6" r:id="rId28" xr:uid="{2D9E69D8-455E-450E-AEF6-CD9BCAA5B209}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
shipment related code for API
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API/GoldApiTestData.xlsx
+++ b/src/test/resources/TestData/API/GoldApiTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C16701-11FE-484D-BA89-4E49819F9D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887CA671-BF9B-4308-A661-6EBA7E5833EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="2496" windowWidth="17280" windowHeight="9108" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="208">
   <si>
     <t>UserName</t>
   </si>
@@ -637,13 +637,22 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>Ship Items</t>
+  </si>
+  <si>
+    <t>https://na-preprod.hele.digital/rest/all/V1/order/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,6 +717,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -742,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -760,6 +776,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1047,19 +1064,19 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1120,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1117,7 +1134,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1132,7 +1149,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1142,63 +1159,63 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="6"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" s="7"/>
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
@@ -1220,33 +1237,33 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="12.6640625" customWidth="1"/>
-    <col min="18" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="11" customWidth="1"/>
-    <col min="36" max="36" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.44140625" customWidth="1"/>
-    <col min="43" max="43" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.42578125" customWidth="1"/>
+    <col min="43" max="43" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1397,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1443,7 +1460,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1466,7 +1483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1474,7 +1491,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -1482,7 +1499,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1496,7 +1513,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1510,7 +1527,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1524,7 +1541,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1538,7 +1555,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1571,7 +1588,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1609,7 +1626,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1623,7 +1640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1639,7 +1656,7 @@
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1670,7 +1687,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1702,7 +1719,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1761,7 +1778,7 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="5"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1818,7 +1835,7 @@
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1830,7 +1847,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1838,7 +1855,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -1855,7 +1872,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1863,7 +1880,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1877,7 +1894,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1894,7 +1911,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1908,7 +1925,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1925,7 +1942,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -1960,28 +1977,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C559D8FD-F843-407C-919F-478081CBDB61}">
-  <dimension ref="A1:AQ34"/>
+  <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="60.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="60.88671875" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="60.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2112,7 +2129,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2175,7 +2192,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>180</v>
       </c>
@@ -2207,7 +2224,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -2237,7 +2254,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -2273,7 +2290,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -2305,26 +2322,24 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>141</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>192</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="17" t="s">
+        <v>206</v>
+      </c>
       <c r="H7" s="2" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="2"/>
       <c r="M7" s="7"/>
       <c r="N7" s="2"/>
@@ -2339,18 +2354,22 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>191</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="2"/>
@@ -2369,162 +2388,174 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" t="s">
-        <v>155</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
-      <c r="AE9" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG9" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI9" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" t="s">
-        <v>161</v>
-      </c>
-      <c r="S10" t="s">
-        <v>32</v>
-      </c>
-      <c r="T10" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="P10" t="s">
+        <v>155</v>
       </c>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
-      <c r="Y10" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ10" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AE10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG10" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI10" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="T11" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+      <c r="S11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" t="s">
+        <v>43</v>
+      </c>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="Y11" s="2"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AJ11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="Y11" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T12" s="2"/>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
-      <c r="AK12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM12">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="Y12" s="2"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AJ12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
       <c r="AK13" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AM13">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
       <c r="X14" s="9"/>
       <c r="AK14" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL14" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AM14">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="AK15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>50</v>
@@ -2533,125 +2564,87 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="T16" s="2"/>
+        <v>55</v>
+      </c>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
-      <c r="Y16" s="2"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AJ16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AK16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM16">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="T17" s="8"/>
+      <c r="E17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T17" s="2"/>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
-      <c r="Y17" s="8"/>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="Y17" s="2"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AJ17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="S18" t="s">
-        <v>32</v>
-      </c>
-      <c r="T18" t="s">
-        <v>43</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="T18" s="8"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="9"/>
-      <c r="Y18" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>168</v>
-      </c>
-      <c r="AB18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD18" s="3"/>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="Y18" s="8"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
+        <v>74</v>
+      </c>
       <c r="S19" t="s">
         <v>32</v>
       </c>
@@ -2663,37 +2656,34 @@
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
       <c r="Y19" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="Z19" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="AA19" t="s">
-        <v>78</v>
+        <v>168</v>
       </c>
       <c r="AB19" s="3" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="AC19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AD19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="5"/>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="7" t="s">
@@ -2722,266 +2712,293 @@
       <c r="W20" s="9"/>
       <c r="X20" s="9"/>
       <c r="Y20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="Z20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AA20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AB20" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AC20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AG20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="5"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" t="s">
+        <v>32</v>
+      </c>
+      <c r="T21" t="s">
+        <v>43</v>
       </c>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
-      <c r="AE21" t="s">
-        <v>171</v>
-      </c>
-      <c r="AG21" s="3"/>
-      <c r="AI21" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="Y21" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="X22" s="9"/>
-      <c r="AJ22" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE22" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG22" s="3"/>
+      <c r="AI22" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>173</v>
-      </c>
-      <c r="S23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T23" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
       <c r="X23" s="9"/>
-      <c r="AN23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>92</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>173</v>
+      </c>
+      <c r="S24" t="s">
+        <v>32</v>
+      </c>
+      <c r="T24" t="s">
+        <v>43</v>
       </c>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
       <c r="X24" s="9"/>
-      <c r="AI24" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AN24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="N25" t="s">
-        <v>97</v>
-      </c>
-      <c r="O25" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q25" s="3"/>
-      <c r="R25" t="s">
-        <v>174</v>
+        <v>42</v>
       </c>
       <c r="U25" s="9"/>
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AI25" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
-      </c>
-      <c r="P26" t="s">
+        <v>97</v>
+      </c>
+      <c r="N26" t="s">
+        <v>97</v>
+      </c>
+      <c r="O26" t="s">
+        <v>29</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="Q26" t="s">
-        <v>175</v>
-      </c>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" t="s">
+        <v>174</v>
+      </c>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="P27" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>175</v>
+      </c>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
-      <c r="AO27" t="s">
-        <v>176</v>
-      </c>
-      <c r="AP27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="9"/>
-      <c r="AE28" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>123</v>
+      <c r="AO28" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>121</v>
       </c>
       <c r="U29" s="9"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
       <c r="AE29" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="P30" t="s">
-        <v>155</v>
-      </c>
-      <c r="S30" t="s">
-        <v>32</v>
-      </c>
-      <c r="T30" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
-      <c r="Y30" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB30" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD30" s="3">
-        <v>888888</v>
-      </c>
-      <c r="AF30" s="12">
-        <v>32725</v>
-      </c>
-      <c r="AK30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM30">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE30" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>62</v>
+        <v>124</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P31" t="s">
+        <v>155</v>
+      </c>
+      <c r="S31" t="s">
+        <v>32</v>
+      </c>
+      <c r="T31" t="s">
+        <v>31</v>
       </c>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="Y31" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB31" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>888888</v>
+      </c>
+      <c r="AF31" s="12">
+        <v>32725</v>
+      </c>
+      <c r="AK31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM31">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="U32" s="9"/>
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
+        <v>126</v>
+      </c>
       <c r="U33" s="9"/>
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>143</v>
@@ -2995,64 +3012,97 @@
       <c r="E34" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="S34" t="s">
+      <c r="F34" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="9"/>
+      <c r="X34" s="9"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="S35" t="s">
         <v>87</v>
       </c>
-      <c r="T34" t="s">
+      <c r="T35" t="s">
         <v>39</v>
       </c>
-      <c r="U34" s="9" t="s">
+      <c r="U35" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="V34" s="9" t="s">
+      <c r="V35" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="W34" s="14">
+      <c r="W35" s="14">
         <v>4</v>
       </c>
-      <c r="X34" t="s">
+      <c r="X35" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D8EBB8AF-0E4E-43B7-9BD6-9022D3DBD128}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
-    <hyperlink ref="C30" r:id="rId4" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
-    <hyperlink ref="E34" r:id="rId5" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
-    <hyperlink ref="D34" r:id="rId6" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
-    <hyperlink ref="C34" r:id="rId7" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
-    <hyperlink ref="B34" r:id="rId8" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
-    <hyperlink ref="E33" r:id="rId9" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
-    <hyperlink ref="D33" r:id="rId10" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
-    <hyperlink ref="C33" r:id="rId11" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
-    <hyperlink ref="B33" r:id="rId12" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
+    <hyperlink ref="B18" r:id="rId3" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
+    <hyperlink ref="C31" r:id="rId4" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
+    <hyperlink ref="E35" r:id="rId5" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
+    <hyperlink ref="D35" r:id="rId6" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
+    <hyperlink ref="C35" r:id="rId7" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
+    <hyperlink ref="B35" r:id="rId8" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
+    <hyperlink ref="E34" r:id="rId9" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
+    <hyperlink ref="D34" r:id="rId10" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
+    <hyperlink ref="C34" r:id="rId11" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
+    <hyperlink ref="B34" r:id="rId12" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
     <hyperlink ref="D2" r:id="rId13" display="testersemail.278@gmail.com" xr:uid="{353015EC-BFE3-4FB0-A1D6-8368DFF2AD28}"/>
-    <hyperlink ref="C19" r:id="rId14" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
-    <hyperlink ref="B19" r:id="rId15" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
-    <hyperlink ref="E20" r:id="rId16" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
-    <hyperlink ref="F17" r:id="rId17" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
-    <hyperlink ref="C17" r:id="rId18" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
-    <hyperlink ref="C16" r:id="rId19" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
+    <hyperlink ref="C20" r:id="rId14" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
+    <hyperlink ref="B20" r:id="rId15" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
+    <hyperlink ref="C18" r:id="rId18" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
+    <hyperlink ref="C17" r:id="rId19" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
     <hyperlink ref="C2" r:id="rId20" display="testersemail.278@gmail.com" xr:uid="{C7FCAAA6-C5F4-4E23-BEE6-5E2DBC6AF4FF}"/>
     <hyperlink ref="F2" r:id="rId21" xr:uid="{8FE9EB04-F6C1-4AA9-8202-6D18E322DE03}"/>
     <hyperlink ref="E2" r:id="rId22" xr:uid="{16136D4B-E0DF-4DB2-B4D1-ABF0F2B7CA08}"/>
     <hyperlink ref="B2" r:id="rId23" xr:uid="{16F2B5CD-2E1E-47F3-B21F-B0588CAC3B53}"/>
     <hyperlink ref="J5" r:id="rId24" display="https://na-preprod.hele.digital/rest/V1/integration/admin/token" xr:uid="{B8077304-30B9-4A5C-85B3-A0C1F75FD2D9}"/>
-    <hyperlink ref="B7" r:id="rId25" xr:uid="{3B86B051-3E41-4698-9B88-E4A853158AAD}"/>
-    <hyperlink ref="H7" r:id="rId26" xr:uid="{3EC40F05-66F6-4B2B-8CD2-3C51732A9D4D}"/>
-    <hyperlink ref="H8" r:id="rId27" xr:uid="{C892FDEA-8590-4AC0-9C8F-5B938B91B017}"/>
+    <hyperlink ref="B8" r:id="rId25" xr:uid="{3B86B051-3E41-4698-9B88-E4A853158AAD}"/>
+    <hyperlink ref="H8" r:id="rId26" xr:uid="{3EC40F05-66F6-4B2B-8CD2-3C51732A9D4D}"/>
+    <hyperlink ref="H9" r:id="rId27" xr:uid="{C892FDEA-8590-4AC0-9C8F-5B938B91B017}"/>
     <hyperlink ref="H6" r:id="rId28" xr:uid="{2D9E69D8-455E-450E-AEF6-CD9BCAA5B209}"/>
+    <hyperlink ref="H7" r:id="rId29" xr:uid="{423F6B9D-BE30-4E13-8A63-3F63117D79F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Invoice code for API
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API/GoldApiTestData.xlsx
+++ b/src/test/resources/TestData/API/GoldApiTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887CA671-BF9B-4308-A661-6EBA7E5833EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1320AF25-4B47-4971-A352-179E6502414C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="210">
   <si>
     <t>UserName</t>
   </si>
@@ -646,6 +646,12 @@
   </si>
   <si>
     <t>https://na-preprod.hele.digital/rest/all/V1/order/</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>https://na-preprod.hele.digital/rest/ospreyusen/V1/order/</t>
   </si>
 </sst>
 </file>
@@ -1977,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C559D8FD-F843-407C-919F-478081CBDB61}">
-  <dimension ref="A1:AQ35"/>
+  <dimension ref="A1:AQ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,7 +1996,9 @@
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="60.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="60.85546875" customWidth="1"/>
     <col min="13" max="13" width="17.28515625" customWidth="1"/>
@@ -2356,24 +2364,22 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>141</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>192</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="17" t="s">
+        <v>208</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="2"/>
       <c r="M8" s="7"/>
       <c r="N8" s="2"/>
@@ -2390,16 +2396,20 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>191</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="2"/>
@@ -2420,160 +2430,172 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="P10" t="s">
-        <v>155</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
-      <c r="AE10" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG10" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI10" s="3" t="s">
-        <v>193</v>
-      </c>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11" t="s">
-        <v>161</v>
-      </c>
-      <c r="S11" t="s">
-        <v>32</v>
-      </c>
-      <c r="T11" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="P11" t="s">
+        <v>155</v>
       </c>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="Y11" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
-        <v>162</v>
+      <c r="AE11" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="T12" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" t="s">
+        <v>161</v>
+      </c>
+      <c r="S12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T12" t="s">
+        <v>43</v>
+      </c>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
-      <c r="Y12" s="2"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AJ12" t="s">
-        <v>164</v>
+      <c r="Y12" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ12" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T13" s="2"/>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
-      <c r="AK13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM13">
-        <v>123</v>
+      <c r="Y13" s="2"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AJ13" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
       <c r="X14" s="9"/>
       <c r="AK14" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AL14" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AM14">
-        <v>1234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="AK15" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AM15">
-        <v>123</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
       <c r="AK16" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AL16" s="5" t="s">
         <v>50</v>
@@ -2584,123 +2606,85 @@
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="T17" s="2"/>
+        <v>55</v>
+      </c>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
-      <c r="Y17" s="2"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AJ17" t="s">
-        <v>165</v>
+      <c r="AK17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM17">
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="T18" s="8"/>
+      <c r="E18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T18" s="2"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="9"/>
-      <c r="Y18" s="8"/>
+      <c r="Y18" s="2"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AJ18" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="S19" t="s">
-        <v>32</v>
-      </c>
-      <c r="T19" t="s">
-        <v>43</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="T19" s="8"/>
       <c r="U19" s="9"/>
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
-      <c r="Y19" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>168</v>
-      </c>
-      <c r="AB19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD19" s="3"/>
+      <c r="Y19" s="8"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
+        <v>74</v>
+      </c>
       <c r="S20" t="s">
         <v>32</v>
       </c>
@@ -2712,37 +2696,34 @@
       <c r="W20" s="9"/>
       <c r="X20" s="9"/>
       <c r="Y20" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="Z20" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="AA20" t="s">
-        <v>78</v>
+        <v>168</v>
       </c>
       <c r="AB20" s="3" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="AC20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AD20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="5"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="7" t="s">
@@ -2771,118 +2752,160 @@
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
       <c r="Y21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="Z21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AA21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AC21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
+      <c r="AG21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="5"/>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" t="s">
+        <v>32</v>
+      </c>
+      <c r="T22" t="s">
+        <v>43</v>
       </c>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="X22" s="9"/>
-      <c r="AE22" t="s">
-        <v>171</v>
-      </c>
-      <c r="AG22" s="3"/>
-      <c r="AI22" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="Y22" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
       <c r="X23" s="9"/>
-      <c r="AJ23" s="3" t="s">
-        <v>172</v>
+      <c r="AE23" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG23" s="3"/>
+      <c r="AI23" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>173</v>
-      </c>
-      <c r="S24" t="s">
-        <v>32</v>
-      </c>
-      <c r="T24" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
       <c r="X24" s="9"/>
-      <c r="AN24" t="s">
-        <v>93</v>
+      <c r="AJ24" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>92</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>173</v>
+      </c>
+      <c r="S25" t="s">
+        <v>32</v>
+      </c>
+      <c r="T25" t="s">
+        <v>43</v>
       </c>
       <c r="U25" s="9"/>
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
-      <c r="AI25" s="3" t="s">
-        <v>94</v>
+      <c r="AN25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
-      </c>
-      <c r="N26" t="s">
-        <v>97</v>
-      </c>
-      <c r="O26" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q26" s="3"/>
-      <c r="R26" t="s">
-        <v>174</v>
+        <v>42</v>
       </c>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
+      <c r="AI26" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
-      </c>
-      <c r="P27" t="s">
+        <v>97</v>
+      </c>
+      <c r="N27" t="s">
+        <v>97</v>
+      </c>
+      <c r="O27" t="s">
+        <v>29</v>
+      </c>
+      <c r="P27" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="Q27" t="s">
-        <v>175</v>
-      </c>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" t="s">
+        <v>174</v>
+      </c>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
@@ -2890,106 +2913,114 @@
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="P28" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>175</v>
+      </c>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="9"/>
-      <c r="AO28" t="s">
-        <v>176</v>
-      </c>
-      <c r="AP28" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="U29" s="9"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
-      <c r="AE29" s="11" t="s">
-        <v>177</v>
+      <c r="AO29" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>123</v>
+      <c r="A30" t="s">
+        <v>121</v>
       </c>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
       <c r="AE30" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="P31" t="s">
-        <v>155</v>
-      </c>
-      <c r="S31" t="s">
-        <v>32</v>
-      </c>
-      <c r="T31" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
-      <c r="Y31" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB31" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD31" s="3">
-        <v>888888</v>
-      </c>
-      <c r="AF31" s="12">
-        <v>32725</v>
-      </c>
-      <c r="AK31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM31">
-        <v>123</v>
+      <c r="AE31" s="11" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>62</v>
+        <v>124</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P32" t="s">
+        <v>155</v>
+      </c>
+      <c r="S32" t="s">
+        <v>32</v>
+      </c>
+      <c r="T32" t="s">
+        <v>31</v>
       </c>
       <c r="U32" s="9"/>
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
+      <c r="Y32" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB32" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD32" s="3">
+        <v>888888</v>
+      </c>
+      <c r="AF32" s="12">
+        <v>32725</v>
+      </c>
+      <c r="AK32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM32">
+        <v>123</v>
+      </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="U33" s="9"/>
       <c r="V33" s="9"/>
@@ -2998,31 +3029,8 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
+        <v>126</v>
+      </c>
       <c r="U34" s="9"/>
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
@@ -3030,7 +3038,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>143</v>
@@ -3044,65 +3052,98 @@
       <c r="E35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="S35" t="s">
+      <c r="F35" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="S36" t="s">
         <v>87</v>
       </c>
-      <c r="T35" t="s">
+      <c r="T36" t="s">
         <v>39</v>
       </c>
-      <c r="U35" s="9" t="s">
+      <c r="U36" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="V35" s="9" t="s">
+      <c r="V36" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="W35" s="14">
+      <c r="W36" s="14">
         <v>4</v>
       </c>
-      <c r="X35" t="s">
+      <c r="X36" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D8EBB8AF-0E4E-43B7-9BD6-9022D3DBD128}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
-    <hyperlink ref="B18" r:id="rId3" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
-    <hyperlink ref="C31" r:id="rId4" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
-    <hyperlink ref="E35" r:id="rId5" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
-    <hyperlink ref="D35" r:id="rId6" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
-    <hyperlink ref="C35" r:id="rId7" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
-    <hyperlink ref="B35" r:id="rId8" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
-    <hyperlink ref="E34" r:id="rId9" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
-    <hyperlink ref="D34" r:id="rId10" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
-    <hyperlink ref="C34" r:id="rId11" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
-    <hyperlink ref="B34" r:id="rId12" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{BF0D3291-B527-40C2-853F-BB57395ADF80}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{FFC3D285-4566-43DA-8B61-72264DD79261}"/>
+    <hyperlink ref="C32" r:id="rId4" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{59159388-5445-48C7-A07A-168A07134A62}"/>
+    <hyperlink ref="E36" r:id="rId5" display="mailto:Lotuswave@123" xr:uid="{25371C73-FBF5-4BCD-931A-C1B129BBAD69}"/>
+    <hyperlink ref="D36" r:id="rId6" display="mailto:skatipelli@helenoftroy.com" xr:uid="{87DF7898-E5F4-4CAA-804F-55B658EA8485}"/>
+    <hyperlink ref="C36" r:id="rId7" display="mailto:skatipelli@helenoftroy.com" xr:uid="{08698846-4648-4E55-9E18-19A7C4BB049A}"/>
+    <hyperlink ref="B36" r:id="rId8" display="mailto:skatipelli@helenoftroy.com" xr:uid="{F61DCA50-B682-4632-BAF8-914C797FE675}"/>
+    <hyperlink ref="E35" r:id="rId9" display="mailto:Lotuswave@123" xr:uid="{E9A0768D-B163-4CC0-833A-315C85EC1680}"/>
+    <hyperlink ref="D35" r:id="rId10" display="mailto:skatipelli@helenoftroy.com" xr:uid="{DBFE72B6-2724-4C6C-99A1-2E19E73C7642}"/>
+    <hyperlink ref="C35" r:id="rId11" display="mailto:skatipelli@helenoftroy.com" xr:uid="{9E86BDB1-CE13-4FDE-A1C2-BED84006B4B5}"/>
+    <hyperlink ref="B35" r:id="rId12" display="mailto:skatipelli@helenoftroy.com" xr:uid="{D7EACAC0-6AB3-4A3D-A8C9-A3AB5BB7ACDC}"/>
     <hyperlink ref="D2" r:id="rId13" display="testersemail.278@gmail.com" xr:uid="{353015EC-BFE3-4FB0-A1D6-8368DFF2AD28}"/>
-    <hyperlink ref="C20" r:id="rId14" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
-    <hyperlink ref="B20" r:id="rId15" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
-    <hyperlink ref="E21" r:id="rId16" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
-    <hyperlink ref="C18" r:id="rId18" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
-    <hyperlink ref="C17" r:id="rId19" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
+    <hyperlink ref="C21" r:id="rId14" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{403A0633-061F-424C-87DD-AE7E0B7C5436}"/>
+    <hyperlink ref="B21" r:id="rId15" display="mailto:lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{90E4E055-93EF-42AC-AF48-4BEC9BB5877F}"/>
+    <hyperlink ref="E22" r:id="rId16" xr:uid="{8F6EB78F-43A3-49AB-919A-9A6934F9A7D4}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{26D5C3C3-90A6-4311-A501-C2DFD87B6098}"/>
+    <hyperlink ref="C19" r:id="rId18" display="testersemail.278@gmail.com" xr:uid="{2B1BB897-47AA-45B2-B8E8-94116B5D65C6}"/>
+    <hyperlink ref="C18" r:id="rId19" xr:uid="{C15CAB9F-48CD-4437-B847-6D8A43A21CBE}"/>
     <hyperlink ref="C2" r:id="rId20" display="testersemail.278@gmail.com" xr:uid="{C7FCAAA6-C5F4-4E23-BEE6-5E2DBC6AF4FF}"/>
     <hyperlink ref="F2" r:id="rId21" xr:uid="{8FE9EB04-F6C1-4AA9-8202-6D18E322DE03}"/>
     <hyperlink ref="E2" r:id="rId22" xr:uid="{16136D4B-E0DF-4DB2-B4D1-ABF0F2B7CA08}"/>
     <hyperlink ref="B2" r:id="rId23" xr:uid="{16F2B5CD-2E1E-47F3-B21F-B0588CAC3B53}"/>
     <hyperlink ref="J5" r:id="rId24" display="https://na-preprod.hele.digital/rest/V1/integration/admin/token" xr:uid="{B8077304-30B9-4A5C-85B3-A0C1F75FD2D9}"/>
-    <hyperlink ref="B8" r:id="rId25" xr:uid="{3B86B051-3E41-4698-9B88-E4A853158AAD}"/>
-    <hyperlink ref="H8" r:id="rId26" xr:uid="{3EC40F05-66F6-4B2B-8CD2-3C51732A9D4D}"/>
-    <hyperlink ref="H9" r:id="rId27" xr:uid="{C892FDEA-8590-4AC0-9C8F-5B938B91B017}"/>
+    <hyperlink ref="B9" r:id="rId25" xr:uid="{3B86B051-3E41-4698-9B88-E4A853158AAD}"/>
+    <hyperlink ref="H9" r:id="rId26" xr:uid="{3EC40F05-66F6-4B2B-8CD2-3C51732A9D4D}"/>
+    <hyperlink ref="H10" r:id="rId27" xr:uid="{C892FDEA-8590-4AC0-9C8F-5B938B91B017}"/>
     <hyperlink ref="H6" r:id="rId28" xr:uid="{2D9E69D8-455E-450E-AEF6-CD9BCAA5B209}"/>
     <hyperlink ref="H7" r:id="rId29" xr:uid="{423F6B9D-BE30-4E13-8A63-3F63117D79F2}"/>
+    <hyperlink ref="H8" r:id="rId30" xr:uid="{82C7216E-7647-4446-AA24-EDFD3120F763}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>